<commit_message>
Adicionado a documentacao de forma correta
</commit_message>
<xml_diff>
--- a/SENAI_HROADS_TARDE_Chris&Bruno/SENAI_HROADS_TARDE_Chris&Bruno.xlsx
+++ b/SENAI_HROADS_TARDE_Chris&Bruno/SENAI_HROADS_TARDE_Chris&Bruno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\OneDrive\Desktop\exercicios-bd-sprint1\exercicios-sprint-1-bd\SENAI_HROADS_TARDE_Chris&amp;Bruno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352FC6CE-6C7A-46FA-AD1B-8E232E44FA19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5229A1A3-A36E-4F87-B563-24450F2F5C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60257C66-3D32-4114-B398-E7816CA5F066}"/>
   </bookViews>
@@ -724,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F11DE7-5A11-4FB0-93E2-367AD14F94F2}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
     <col min="19" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -760,7 +760,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -783,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>10</v>
       </c>
@@ -806,7 +806,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>15</v>
       </c>
@@ -829,7 +829,7 @@
         <v>42446</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>20</v>
       </c>
@@ -852,8 +852,8 @@
         <v>43177</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
@@ -862,17 +862,8 @@
         <v>4</v>
       </c>
       <c r="E8" s="24"/>
-      <c r="G8" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-      <c r="K8" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="44"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
@@ -885,23 +876,8 @@
       <c r="E9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -914,23 +890,8 @@
       <c r="E10" s="28">
         <v>4</v>
       </c>
-      <c r="G10" s="37">
-        <v>4</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="39">
-        <v>90</v>
-      </c>
-      <c r="K10" s="47">
-        <v>90</v>
-      </c>
-      <c r="L10" s="48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>2</v>
       </c>
@@ -943,23 +904,8 @@
       <c r="E11" s="28">
         <v>6</v>
       </c>
-      <c r="G11" s="37">
-        <v>5</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="39">
-        <v>95</v>
-      </c>
-      <c r="K11" s="47">
-        <v>95</v>
-      </c>
-      <c r="L11" s="48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>3</v>
       </c>
@@ -972,23 +918,8 @@
       <c r="E12" s="28">
         <v>5</v>
       </c>
-      <c r="G12" s="40">
-        <v>6</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="42">
-        <v>100</v>
-      </c>
-      <c r="K12" s="49">
-        <v>100</v>
-      </c>
-      <c r="L12" s="50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>4</v>
       </c>
@@ -1002,7 +933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>5</v>
       </c>
@@ -1010,7 +941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>6</v>
       </c>
@@ -1018,12 +949,92 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <v>7</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="D19" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="47">
+        <v>90</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="37">
+        <v>4</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="39">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="47">
+        <v>95</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="37">
+        <v>5</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="39">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49">
+        <v>100</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="40">
+        <v>6</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="42">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>